<commit_message>
[ADD]: se añadio el author al scraping
</commit_message>
<xml_diff>
--- a/articulos-mozilla.xlsx
+++ b/articulos-mozilla.xlsx
@@ -427,7 +427,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Autor no encontrado</v>
+        <v>Haik Aftandilian</v>
       </c>
       <c r="B2" t="str">
         <v>Improving Firefox Stability in the Enterprise by Reducing DLL Injection</v>
@@ -450,7 +450,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Autor no encontrado</v>
+        <v>James Graham</v>
       </c>
       <c r="B3" t="str">
         <v>Launching Interop 2025</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Autor no encontrado</v>
+        <v>Mark Mayo</v>
       </c>
       <c r="B4" t="str">
         <v>Introducing Uniffi for React Native: Rust-Powered Turbo Modules</v>
@@ -496,7 +496,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Autor no encontrado</v>
+        <v>Stephen Hood</v>
       </c>
       <c r="B5" t="str">
         <v>Llamafile v0.8.14: a new UI, performance gains, and more</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Autor no encontrado</v>
+        <v>Marco Figueroa</v>
       </c>
       <c r="B6" t="str">
         <v>0Din: A GenAI Bug Bounty Program – Securing Tomorrow’s AI Together</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Autor no encontrado</v>
+        <v>James Graham</v>
       </c>
       <c r="B7" t="str">
         <v>Announcing Official Puppeteer Support for Firefox</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Autor no encontrado</v>
+        <v>Christian Holler</v>
       </c>
       <c r="B8" t="str">
         <v>Snapshots for IPC Fuzzing</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Autor no encontrado</v>
+        <v>Stephen Hood</v>
       </c>
       <c r="B9" t="str">
         <v>Sponsoring sqlite-vec to enable more powerful Local AI applications</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Autor no encontrado</v>
+        <v>Tarek Ziadé</v>
       </c>
       <c r="B10" t="str">
         <v>Experimenting with local alt text generation in Firefox Nightly</v>
@@ -634,7 +634,7 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Autor no encontrado</v>
+        <v>Stephen Hood</v>
       </c>
       <c r="B11" t="str">
         <v>Llamafile’s progress, four months in</v>
@@ -657,7 +657,7 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Autor no encontrado</v>
+        <v>Alex Franchuk</v>
       </c>
       <c r="B12" t="str">
         <v>Porting a cross-platform GUI application to Rust</v>
@@ -680,7 +680,7 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Autor no encontrado</v>
+        <v>Thomas Lodato</v>
       </c>
       <c r="B13" t="str">
         <v>Prototype even faster with the Gradio UI for Figma component library</v>
@@ -703,7 +703,7 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Autor no encontrado</v>
+        <v>Brian Grinstead</v>
       </c>
       <c r="B14" t="str">
         <v>Improving Performance in Firefox and Across the Web with Speedometer 3</v>
@@ -726,7 +726,7 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Autor no encontrado</v>
+        <v>James Graham</v>
       </c>
       <c r="B15" t="str">
         <v>Announcing Interop 2024</v>
@@ -749,7 +749,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Autor no encontrado</v>
+        <v>Serge Guelton</v>
       </c>
       <c r="B16" t="str">
         <v>Option Soup: the subtle pitfalls of combining compiler flags</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Autor no encontrado</v>
+        <v>James Graham</v>
       </c>
       <c r="B17" t="str">
         <v>Puppeteer Support for the Cross-Browser WebDriver BiDi Standard</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Autor no encontrado</v>
+        <v>Johan Lorenzo (Mozilla)</v>
       </c>
       <c r="B18" t="str">
         <v>Firefox Developer Edition and Beta: Try out Mozilla’s .deb package!</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Autor no encontrado</v>
+        <v>Stephen Hood</v>
       </c>
       <c r="B19" t="str">
         <v>Introducing llamafile</v>
@@ -841,7 +841,7 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Autor no encontrado</v>
+        <v>Dan Brown</v>
       </c>
       <c r="B20" t="str">
         <v>Mozilla AI Guide Launch with Summarization Code Example</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Autor no encontrado</v>
+        <v>Bas Schouten</v>
       </c>
       <c r="B21" t="str">
         <v>Down and to the Right: Firefox Got Faster for Real Users in 2023</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Autor no encontrado</v>
+        <v>Bobby Holley</v>
       </c>
       <c r="B22" t="str">
         <v>Built for Privacy: Partnering to Deploy Oblivious HTTP and Prio in Firefox</v>
@@ -910,7 +910,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Autor no encontrado</v>
+        <v>Brian Grinstead</v>
       </c>
       <c r="B23" t="str">
         <v>Faster Vue.js Execution in Firefox</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Autor no encontrado</v>
+        <v>Ben Dean-Kawamura</v>
       </c>
       <c r="B24" t="str">
         <v>Autogenerating Rust-JS bindings with UniFFI</v>
@@ -956,7 +956,7 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>Autor no encontrado</v>
+        <v>Stephen Hood</v>
       </c>
       <c r="B25" t="str">
         <v>So you want to build your own open source ChatGPT-style chatbot…</v>
@@ -979,7 +979,7 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Autor no encontrado</v>
+        <v>Greg Stoll</v>
       </c>
       <c r="B26" t="str">
         <v>Letting users block injected third-party DLLs in Firefox</v>
@@ -1002,7 +1002,7 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Autor no encontrado</v>
+        <v>Dan Brown</v>
       </c>
       <c r="B27" t="str">
         <v>Mozilla Launches Responsible AI Challenge</v>
@@ -1025,7 +1025,7 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Autor no encontrado</v>
+        <v>James Graham</v>
       </c>
       <c r="B28" t="str">
         <v>Announcing Interop 2023</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>Autor no encontrado</v>
+        <v>James Graham</v>
       </c>
       <c r="B29" t="str">
         <v>Interop 2022: Outcomes</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>Autor no encontrado</v>
+        <v>Francesca Minelli</v>
       </c>
       <c r="B30" t="str">
         <v>How the Mozilla Community helps shape our products</v>
@@ -1094,7 +1094,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Autor no encontrado</v>
+        <v>Gabriele Svelto</v>
       </c>
       <c r="B31" t="str">
         <v>Improving Firefox stability with this one weird trick</v>

</xml_diff>